<commit_message>
feat(location) : rules replace
</commit_message>
<xml_diff>
--- a/output/zy-3月第4周周报.xlsx
+++ b/output/zy-3月第4周周报.xlsx
@@ -13,9 +13,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
-  <si>
-    <t>qd周报（{month}月）</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+  <si>
+    <t>qd周报（3月）</t>
   </si>
   <si>
     <t>日期：2018年3月14日-2018年3月16日</t>
@@ -42,7 +42,19 @@
     <t>下周主要事项</t>
   </si>
   <si>
-    <t>null</t>
+    <t>c</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
   <si>
     <t>本周工作记录</t>
@@ -98,7 +110,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <name val="宋体"/>
       <color indexed="8"/>
@@ -141,10 +153,6 @@
     <font>
       <name val="微软雅黑"/>
       <color indexed="8"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <color rgb="00000000"/>
       <sz val="12"/>
     </font>
   </fonts>
@@ -278,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -286,10 +294,10 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="3" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -298,95 +306,86 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="5" fontId="5" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="3" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="6" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="4" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="6" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="6" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="5" fontId="5" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="6" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="7" numFmtId="56" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="6" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="6" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="6" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="6" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="6" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="6" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="4" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="6" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="6" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="4" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="5" fillId="7" fontId="8" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="7" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="5" fillId="7" fontId="8" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="7" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="7" fontId="8" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="7" fontId="8" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="7" fontId="8" numFmtId="56" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="7" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="7" fontId="8" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="7" fontId="8" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="5" fillId="7" fontId="3" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="5" fillId="7" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="7" fontId="5" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="7" fontId="6" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="7" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="7" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="7" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="7" fontId="7" numFmtId="56" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="7" fontId="6" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1463,7 +1462,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="11" defaultRowHeight="18" outlineLevelCol="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="11" defaultRowHeight="14" outlineLevelCol="0" outlineLevelRow="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="1" width="9.351559999999999"/>
     <col customWidth="1" max="2" min="2" style="1" width="10.6719"/>
@@ -1474,313 +1473,313 @@
     <col customWidth="1" max="256" min="7" style="1" width="11"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="43" r="1" s="27" spans="1:6">
-      <c r="A1" s="28" t="s">
+    <row customHeight="1" ht="43" r="1" s="23" spans="1:6">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="n"/>
-      <c r="C1" s="29" t="n"/>
-      <c r="D1" s="29" t="n"/>
-      <c r="E1" s="29" t="n"/>
-      <c r="F1" s="29" t="n"/>
-    </row>
-    <row customHeight="1" ht="32" r="2" s="27" spans="1:6">
-      <c r="A2" s="30" t="s">
+      <c r="B1" s="25" t="n"/>
+      <c r="C1" s="25" t="n"/>
+      <c r="D1" s="25" t="n"/>
+      <c r="E1" s="25" t="n"/>
+      <c r="F1" s="25" t="n"/>
+    </row>
+    <row customHeight="1" ht="32" r="2" s="23" spans="1:6">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="n"/>
-      <c r="C2" s="29" t="n"/>
-      <c r="D2" s="30" t="s">
+      <c r="B2" s="25" t="n"/>
+      <c r="C2" s="25" t="n"/>
+      <c r="D2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="29" t="n"/>
-      <c r="F2" s="30" t="s">
+      <c r="E2" s="25" t="n"/>
+      <c r="F2" s="26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row customHeight="1" ht="32" r="3" s="27" spans="1:6">
-      <c r="A3" s="28" t="s">
+    <row customHeight="1" ht="32" r="3" s="23" spans="1:6">
+      <c r="A3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="29" t="n"/>
-      <c r="C3" s="29" t="n"/>
-      <c r="D3" s="28" t="s">
+      <c r="B3" s="25" t="n"/>
+      <c r="C3" s="25" t="n"/>
+      <c r="D3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="29" t="n"/>
-      <c r="F3" s="29" t="n"/>
-    </row>
-    <row customHeight="1" ht="26" r="4" s="27" spans="1:6">
+      <c r="E3" s="25" t="n"/>
+      <c r="F3" s="25" t="n"/>
+    </row>
+    <row customHeight="1" ht="26" r="4" s="23" spans="1:6">
       <c r="A4" s="28" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="29" t="n"/>
+      <c r="C4" s="25" t="n"/>
       <c r="D4" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="29" t="n"/>
-    </row>
-    <row customHeight="1" ht="31" r="5" s="27" spans="1:6">
-      <c r="A5" s="31" t="n">
+      <c r="F4" s="25" t="n"/>
+    </row>
+    <row customHeight="1" ht="31" r="5" s="23" spans="1:6">
+      <c r="A5" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="29" t="n"/>
-      <c r="D5" s="31" t="n">
+      <c r="C5" s="25" t="n"/>
+      <c r="D5" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="29" t="n"/>
-    </row>
-    <row customHeight="1" ht="31" r="6" s="27" spans="1:6">
-      <c r="A6" s="31" t="n">
+      <c r="E5" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="25" t="n"/>
+    </row>
+    <row customHeight="1" ht="31" r="6" s="23" spans="1:6">
+      <c r="A6" s="29" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="29" t="n"/>
-      <c r="D6" s="31" t="n">
+      <c r="B6" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="25" t="n"/>
+      <c r="D6" s="29" t="n">
         <v>2</v>
       </c>
-      <c r="E6" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="29" t="n"/>
-    </row>
-    <row customHeight="1" ht="31" r="7" s="27" spans="1:6">
-      <c r="A7" s="31" t="n">
+      <c r="E6" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="25" t="n"/>
+    </row>
+    <row customHeight="1" ht="31" r="7" s="23" spans="1:6">
+      <c r="A7" s="29" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="29" t="n"/>
-      <c r="D7" s="31" t="n">
+      <c r="B7" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="25" t="n"/>
+      <c r="D7" s="29" t="n">
         <v>3</v>
       </c>
-      <c r="E7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="29" t="n"/>
-    </row>
-    <row customHeight="1" ht="26" r="8" s="27" spans="1:6">
-      <c r="A8" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="29" t="n"/>
-      <c r="C8" s="29" t="n"/>
-      <c r="D8" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="29" t="n"/>
-      <c r="F8" s="29" t="n"/>
-    </row>
-    <row customHeight="1" ht="23" r="9" s="27" spans="1:6">
+      <c r="E7" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="25" t="n"/>
+    </row>
+    <row customHeight="1" ht="26" r="8" s="23" spans="1:6">
+      <c r="A8" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="25" t="n"/>
+      <c r="C8" s="25" t="n"/>
+      <c r="D8" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="25" t="n"/>
+      <c r="F8" s="25" t="n"/>
+    </row>
+    <row customHeight="1" ht="23" r="9" s="23" spans="1:6">
       <c r="A9" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="29" t="n"/>
+        <v>16</v>
+      </c>
+      <c r="B9" s="25" t="n"/>
       <c r="C9" s="28" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F9" s="28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="62.25" r="10" s="23" spans="1:6">
+      <c r="A10" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="32" t="n">
+        <v>43171</v>
+      </c>
+      <c r="C10" s="33" t="n"/>
+      <c r="D10" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="33" t="n"/>
+      <c r="F10" s="33" t="n"/>
+    </row>
+    <row customHeight="1" ht="59.25" r="11" s="23" spans="1:6">
+      <c r="A11" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="32" t="n">
+        <v>43172</v>
+      </c>
+      <c r="C11" s="33" t="n"/>
+      <c r="D11" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="33" t="n"/>
+      <c r="F11" s="33" t="n"/>
+    </row>
+    <row customHeight="1" ht="51.75" r="12" s="23" spans="1:6">
+      <c r="A12" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="32" t="n">
+        <v>43173</v>
+      </c>
+      <c r="C12" s="30" t="n"/>
+      <c r="D12" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" s="33" t="n"/>
+      <c r="F12" s="33" t="n"/>
+    </row>
+    <row customHeight="1" ht="51.75" r="13" s="23" spans="1:6">
+      <c r="A13" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="32" t="n">
+        <v>43174</v>
+      </c>
+      <c r="C13" s="30" t="n"/>
+      <c r="D13" s="29" t="n"/>
+      <c r="E13" s="33" t="n"/>
+      <c r="F13" s="33" t="n"/>
+    </row>
+    <row customHeight="1" ht="59.25" r="14" s="23" spans="1:6">
+      <c r="A14" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="32" t="n">
+        <v>43175</v>
+      </c>
+      <c r="C14" s="30" t="n"/>
+      <c r="D14" s="29" t="n"/>
+      <c r="E14" s="33" t="n"/>
+      <c r="F14" s="33" t="n"/>
+    </row>
+    <row customHeight="1" ht="26" r="15" s="23" spans="1:6">
+      <c r="A15" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="25" t="n"/>
+      <c r="C15" s="25" t="n"/>
+      <c r="D15" s="25" t="n"/>
+      <c r="E15" s="25" t="n"/>
+      <c r="F15" s="25" t="n"/>
+    </row>
+    <row customHeight="1" ht="30" r="16" s="23" spans="1:6">
+      <c r="A16" s="28" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row customHeight="1" ht="62.25" r="10" s="27" spans="1:6">
-      <c r="A10" s="28" t="s">
+      <c r="B16" s="25" t="n"/>
+      <c r="C16" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="34" t="n">
-        <v>43171</v>
-      </c>
-      <c r="C10" s="35" t="n"/>
-      <c r="D10" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="35" t="n"/>
-      <c r="F10" s="35" t="n"/>
-    </row>
-    <row customHeight="1" ht="59.25" r="11" s="27" spans="1:6">
-      <c r="A11" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="34" t="n">
-        <v>43172</v>
-      </c>
-      <c r="C11" s="35" t="n"/>
-      <c r="D11" s="31" t="n">
-        <v>2</v>
-      </c>
-      <c r="E11" s="35" t="n"/>
-      <c r="F11" s="35" t="n"/>
-    </row>
-    <row customHeight="1" ht="51.75" r="12" s="27" spans="1:6">
-      <c r="A12" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="34" t="n">
-        <v>43173</v>
-      </c>
-      <c r="C12" s="36" t="n"/>
-      <c r="D12" s="31" t="n">
-        <v>3</v>
-      </c>
-      <c r="E12" s="35" t="n"/>
-      <c r="F12" s="35" t="n"/>
-    </row>
-    <row customHeight="1" ht="51.75" r="13" s="27" spans="1:6">
-      <c r="A13" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="34" t="n">
-        <v>43174</v>
-      </c>
-      <c r="C13" s="36" t="n"/>
-      <c r="D13" s="31" t="n"/>
-      <c r="E13" s="35" t="n"/>
-      <c r="F13" s="35" t="n"/>
-    </row>
-    <row customHeight="1" ht="59.25" r="14" s="27" spans="1:6">
-      <c r="A14" s="28" t="s">
+      <c r="D16" s="25" t="n"/>
+      <c r="E16" s="25" t="n"/>
+      <c r="F16" s="25" t="n"/>
+    </row>
+    <row customHeight="1" ht="57" r="17" s="23" spans="1:6">
+      <c r="A17" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="34" t="n">
-        <v>43175</v>
-      </c>
-      <c r="C14" s="36" t="n"/>
-      <c r="D14" s="31" t="n"/>
-      <c r="E14" s="35" t="n"/>
-      <c r="F14" s="35" t="n"/>
-    </row>
-    <row customHeight="1" ht="26" r="15" s="27" spans="1:6">
-      <c r="A15" s="28" t="s">
+      <c r="B17" s="32" t="n">
+        <v>43115</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="25" t="n"/>
+      <c r="E17" s="25" t="n"/>
+      <c r="F17" s="25" t="n"/>
+    </row>
+    <row customHeight="1" ht="51" r="18" s="23" spans="1:6">
+      <c r="A18" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="29" t="n"/>
-      <c r="C15" s="29" t="n"/>
-      <c r="D15" s="29" t="n"/>
-      <c r="E15" s="29" t="n"/>
-      <c r="F15" s="29" t="n"/>
-    </row>
-    <row customHeight="1" ht="30" r="16" s="27" spans="1:6">
-      <c r="A16" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="29" t="n"/>
-      <c r="C16" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="29" t="n"/>
-      <c r="E16" s="29" t="n"/>
-      <c r="F16" s="29" t="n"/>
-    </row>
-    <row customHeight="1" ht="57" r="17" s="27" spans="1:6">
-      <c r="A17" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="34" t="n">
-        <v>43115</v>
-      </c>
-      <c r="C17" s="36" t="s">
+      <c r="B18" s="32" t="n">
+        <v>43116</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="25" t="n"/>
+      <c r="E18" s="25" t="n"/>
+      <c r="F18" s="25" t="n"/>
+    </row>
+    <row customHeight="1" ht="53.25" r="19" s="23" spans="1:6">
+      <c r="A19" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="29" t="n"/>
-      <c r="E17" s="29" t="n"/>
-      <c r="F17" s="29" t="n"/>
-    </row>
-    <row customHeight="1" ht="51" r="18" s="27" spans="1:6">
-      <c r="A18" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="34" t="n">
-        <v>43116</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="29" t="n"/>
-      <c r="E18" s="29" t="n"/>
-      <c r="F18" s="29" t="n"/>
-    </row>
-    <row customHeight="1" ht="53.25" r="19" s="27" spans="1:6">
-      <c r="A19" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="34" t="n">
+      <c r="B19" s="32" t="n">
         <v>43117</v>
       </c>
-      <c r="C19" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="29" t="n"/>
-      <c r="E19" s="29" t="n"/>
-      <c r="F19" s="29" t="n"/>
-    </row>
-    <row customHeight="1" ht="53.25" r="20" s="27" spans="1:6">
-      <c r="A20" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="34" t="n">
+      <c r="C19" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="25" t="n"/>
+      <c r="E19" s="25" t="n"/>
+      <c r="F19" s="25" t="n"/>
+    </row>
+    <row customHeight="1" ht="53.25" r="20" s="23" spans="1:6">
+      <c r="A20" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="32" t="n">
         <v>43118</v>
       </c>
-      <c r="C20" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="29" t="n"/>
-      <c r="E20" s="29" t="n"/>
-      <c r="F20" s="29" t="n"/>
-    </row>
-    <row customHeight="1" ht="49.5" r="21" s="27" spans="1:6">
-      <c r="A21" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="34" t="n">
+      <c r="C20" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="25" t="n"/>
+      <c r="E20" s="25" t="n"/>
+      <c r="F20" s="25" t="n"/>
+    </row>
+    <row customHeight="1" ht="49.5" r="21" s="23" spans="1:6">
+      <c r="A21" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="32" t="n">
         <v>43119</v>
       </c>
-      <c r="C21" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="29" t="n"/>
-      <c r="E21" s="29" t="n"/>
-      <c r="F21" s="29" t="n"/>
-    </row>
-    <row customHeight="1" ht="30.75" r="22" s="27" spans="1:6">
-      <c r="A22" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="29" t="n"/>
-      <c r="C22" s="35" t="n"/>
-      <c r="D22" s="29" t="n"/>
-      <c r="E22" s="29" t="n"/>
-      <c r="F22" s="29" t="n"/>
-    </row>
-    <row customHeight="1" ht="98.25" r="23" s="27" spans="1:6">
-      <c r="A23" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="29" t="n"/>
-      <c r="C23" s="29" t="n"/>
-      <c r="D23" s="29" t="n"/>
-      <c r="E23" s="29" t="n"/>
-      <c r="F23" s="29" t="n"/>
+      <c r="C21" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="25" t="n"/>
+      <c r="E21" s="25" t="n"/>
+      <c r="F21" s="25" t="n"/>
+    </row>
+    <row customHeight="1" ht="30.75" r="22" s="23" spans="1:6">
+      <c r="A22" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="25" t="n"/>
+      <c r="C22" s="33" t="n"/>
+      <c r="D22" s="25" t="n"/>
+      <c r="E22" s="25" t="n"/>
+      <c r="F22" s="25" t="n"/>
+    </row>
+    <row customHeight="1" ht="98.25" r="23" s="23" spans="1:6">
+      <c r="A23" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="25" t="n"/>
+      <c r="C23" s="25" t="n"/>
+      <c r="D23" s="25" t="n"/>
+      <c r="E23" s="25" t="n"/>
+      <c r="F23" s="25" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="27">

</xml_diff>